<commit_message>
Adding pricing for amazon
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Home\Documents\bawcs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AA3AEB-BEBA-43BE-849E-E385B3775902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4317E4-B8BD-46F0-B0F5-313C440F584B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB65EE7C-7D71-4D9B-ABF7-5CAC2D8EB355}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB65EE7C-7D71-4D9B-ABF7-5CAC2D8EB355}"/>
   </bookViews>
   <sheets>
     <sheet name="Full BOM" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="124">
   <si>
     <t>Part name</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Prototyping Board</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32841816748.html</t>
-  </si>
-  <si>
     <t>300mm 2020 V-Slot Extrusion</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
     <t>https://vilros.com/products/raspberry-pi-zero-wh</t>
   </si>
   <si>
-    <t>Looks nice</t>
-  </si>
-  <si>
     <t>1K Ohm Resistors</t>
   </si>
   <si>
@@ -200,16 +194,16 @@
     <t>NEMA17 T8*8 Lead Screw Stepper Motor</t>
   </si>
   <si>
+    <t>UV Film</t>
+  </si>
+  <si>
     <t>N52 12mmx3mm Magnets</t>
   </si>
   <si>
     <t>https://www.ebay.com/i/293052139246?chn=ps&amp;mkevt=1&amp;mkcid=28</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>Yes</t>
   </si>
   <si>
     <t>Front Panel Piece</t>
@@ -230,9 +224,6 @@
     <t>608 Bearings</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32813154852.html</t>
-  </si>
-  <si>
     <t>Delta AFC1212DE-SP02 120x120x38mm Fan</t>
   </si>
   <si>
@@ -240,6 +231,180 @@
   </si>
   <si>
     <t>https://www.ebay.com/c/670506937</t>
+  </si>
+  <si>
+    <t>Alt Quantity</t>
+  </si>
+  <si>
+    <t>Sub Unit Price</t>
+  </si>
+  <si>
+    <t>6x6x6mm Tactile Buttons</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32960657626.html</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/4000911353131.html</t>
+  </si>
+  <si>
+    <t>OBE</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/i/193667517692</t>
+  </si>
+  <si>
+    <t>MCP23017 I2C IO Extender</t>
+  </si>
+  <si>
+    <t>ESP-WROOM-32 NodeMCU</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/i/184310896504</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/4000301371545.html</t>
+  </si>
+  <si>
+    <t>You want a half size one</t>
+  </si>
+  <si>
+    <t>Amazon Quantity</t>
+  </si>
+  <si>
+    <t>Amazon Total Price</t>
+  </si>
+  <si>
+    <t>Alt Link</t>
+  </si>
+  <si>
+    <t>Amazon / What I Used Price</t>
+  </si>
+  <si>
+    <t>More Expensive Link</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0185FGTSS/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0185FIOTA/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B087PVM2NT/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07VT199JR/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07ZYTZ48N/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0776F4BKH/ref=ppx_yo_dt_b_asin_title_o01_s02?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B083XF431P/ref=ppx_yo_dt_b_asin_title_o01_s02?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B01N5VYSES/ref=ppx_yo_dt_b_asin_title_o01_s03?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07T8BSKFP/ref=ppx_yo_dt_b_asin_title_o04_s01?ie=UTF8&amp;th=1</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>2x Set</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B01FFGAKK8/ref=ppx_yo_dt_b_asin_title_o05_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Carbon Filters x6</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07D5SBPN8/ref=ppx_yo_dt_b_asin_title_o09_s01?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B0723BG637/ref=ppx_yo_dt_b_asin_title_o09_s01?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07FQF2BRC/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07N3QT628/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>Same, with Readouts</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07FBZ7NML/ref=ppx_yo_dt_b_asin_title_o05_s00?ie=UTF8&amp;th=1</t>
+  </si>
+  <si>
+    <t>Same, but free shipping</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/Delta-DC-Brushless-12V-y4574-1-6-Amp-4-PIN-Cooling-Fan-120x120x38/273159431365?hash=item3f999224c5:g:~2gAAOSwyGBa0k2H</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/2x1/8 </t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/i/283623299469?chn=ps&amp;mkevt=1&amp;mkcid=28</t>
+  </si>
+  <si>
+    <t>STP16NF06L Logic Level</t>
+  </si>
+  <si>
+    <t>Pack 100</t>
+  </si>
+  <si>
+    <t>Pack 10</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/BOJACK-16Voltage-Aluminum-Electrolytic-Capacitors/dp/B07S7QSVHV</t>
+  </si>
+  <si>
+    <t>Same, watch for bad silkscreen</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Display-Control-Horizontal-Vertical-Adjustment/dp/B07WFCH1H4</t>
+  </si>
+  <si>
+    <t>Same x20 pack</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Sackorange-Skateboard-Bearings-Miniature-Bearings%EF%BC%88Pack/dp/B07216D1SZ/</t>
+  </si>
+  <si>
+    <t>Same x4 pack</t>
+  </si>
+  <si>
+    <t>Same 16ft</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07K6BK639/ref=ppx_yo_dt_b_asin_title_o02_s01?ie=UTF8&amp;psc=1</t>
+  </si>
+  <si>
+    <t>SD Cards x2</t>
+  </si>
+  <si>
+    <t>Pack x4</t>
+  </si>
+  <si>
+    <t>A4988 x5</t>
+  </si>
+  <si>
+    <t>Pack x200</t>
+  </si>
+  <si>
+    <t>Same, basically</t>
   </si>
 </sst>
 </file>
@@ -299,7 +464,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -308,6 +473,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="8" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -340,37 +508,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97BDDAB7-552A-40C5-BAD6-B08585462BC3}" name="Table1" displayName="Table1" ref="A1:G31" totalsRowCount="1">
-  <autoFilter ref="A1:G30" xr:uid="{58634776-3A17-47A1-AF55-6F78625F63F8}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{97BDDAB7-552A-40C5-BAD6-B08585462BC3}" name="Table1" displayName="Table1" ref="A1:P32" totalsRowCount="1">
+  <autoFilter ref="A1:P31" xr:uid="{58634776-3A17-47A1-AF55-6F78625F63F8}"/>
+  <tableColumns count="16">
     <tableColumn id="1" xr3:uid="{6A66FFF7-211A-4D6D-94CA-6AF2C37D313A}" name="Part name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{E77B4F11-A677-4745-8047-C15D89A0CF02}" name="Quantity"/>
     <tableColumn id="3" xr3:uid="{AD27C4C6-F118-4149-AE2B-FEC0FE68A6B7}" name="Substitute"/>
     <tableColumn id="4" xr3:uid="{C32E265C-460F-4D8E-A85A-4C3D94D3993A}" name="Unit Price"/>
-    <tableColumn id="5" xr3:uid="{31FC8869-1D17-4924-9F24-1800F0BA3844}" name="Total" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
-      <calculatedColumnFormula>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{31FC8869-1D17-4924-9F24-1800F0BA3844}" name="Total" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="1">
+      <calculatedColumnFormula>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{BD9159B4-73C3-43E7-8A5A-C6E132B0A2FF}" name="Link"/>
     <tableColumn id="7" xr3:uid="{D142BAD2-AC92-40FE-8028-1061A16739FC}" name="Notes"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{21578413-7310-43D9-8032-BD03C617EAE5}" name="Table2" displayName="Table2" ref="I1:N30" totalsRowShown="0">
-  <autoFilter ref="I1:N30" xr:uid="{0CA2714B-E8C4-4E41-9778-5439AC5A33B8}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{4D17FFB8-13A4-4857-A8EF-C9F223F269EC}" name="Substitute Name"/>
-    <tableColumn id="2" xr3:uid="{E4DDCD4D-D7A9-4ED6-89F1-4ED1014441C0}" name="Quantity"/>
-    <tableColumn id="3" xr3:uid="{B423799A-C68B-4F2A-98B6-70C9196CD869}" name="Unit Price"/>
-    <tableColumn id="4" xr3:uid="{35D951D2-9D64-4163-BF1A-C708BA36627F}" name="Total" dataDxfId="2">
-      <calculatedColumnFormula>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{873DC0F2-E861-4A41-95C3-344FCDECD439}" name="Substitute Name"/>
+    <tableColumn id="9" xr3:uid="{24F632C7-7AC4-43DD-8614-94A808659F47}" name="Alt Quantity"/>
+    <tableColumn id="10" xr3:uid="{14DFBAF5-2668-4DDF-AF37-C9592B3B8772}" name="Sub Unit Price"/>
+    <tableColumn id="11" xr3:uid="{EF38FE59-A0C6-45C6-9C02-635D2C0F8650}" name="Alt Link"/>
+    <tableColumn id="18" xr3:uid="{FF6DA1CE-C149-4CBB-9DC6-16454B4F3251}" name="Description"/>
+    <tableColumn id="12" xr3:uid="{C52948AE-22AA-42D0-B073-EE495448D09D}" name="Amazon / What I Used Price"/>
+    <tableColumn id="13" xr3:uid="{FF337B68-0B19-4F10-8026-0DB82D36583F}" name="Amazon Quantity"/>
+    <tableColumn id="15" xr3:uid="{9E15660B-6288-4FDB-93F5-7A838D513078}" name="Amazon Total Price" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D7F5AB23-24E2-42F8-AD3D-C779F5FDB1E9}" name="Link" dataDxfId="3">
-      <calculatedColumnFormula>Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]]</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{1C29C07D-CFA8-448D-8699-B5206F20EA5D}" name="Notes"/>
+    <tableColumn id="14" xr3:uid="{E0A004EC-E40C-43C4-AFBE-572E4D8251A3}" name="More Expensive Link"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -673,22 +833,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C837E81B-66FE-4A6A-9C4C-66ED9AD70C3B}">
-  <dimension ref="A1:N42"/>
+  <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
     <col min="2" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="56" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.42578125" customWidth="1"/>
     <col min="9" max="14" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -710,26 +871,35 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="K1" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="L1" t="s">
-        <v>4</v>
+        <v>92</v>
       </c>
       <c r="M1" t="s">
-        <v>5</v>
+        <v>81</v>
       </c>
       <c r="N1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="O1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -740,30 +910,30 @@
         <v>8</v>
       </c>
       <c r="E2" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>93</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -771,33 +941,48 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="D3">
+        <v>2.5</v>
       </c>
       <c r="E3" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2">
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>16.28</v>
       </c>
-      <c r="L3" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
+      <c r="H3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
         <v>16.28</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="N3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="2">
+        <v>24.95</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>24.95</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="3"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -808,16 +993,29 @@
         <v>8</v>
       </c>
       <c r="E4" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="L4" t="s">
+        <v>93</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>0</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -828,36 +1026,65 @@
         <v>8</v>
       </c>
       <c r="E5" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" t="s">
+        <v>93</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>0</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>71</v>
+      </c>
+      <c r="D6">
+        <v>2.5</v>
       </c>
       <c r="E6" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>93</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>0</v>
+      </c>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -868,16 +1095,29 @@
         <v>8</v>
       </c>
       <c r="E7" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>0</v>
-      </c>
-      <c r="L7" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="L7" t="s">
+        <v>93</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>0</v>
+      </c>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -888,18 +1128,31 @@
         <v>8</v>
       </c>
       <c r="E8" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>0</v>
-      </c>
-      <c r="L8" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="L8" t="s">
+        <v>93</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>0</v>
+      </c>
+      <c r="U8" s="2"/>
+      <c r="V8" s="2"/>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -911,24 +1164,44 @@
         <v>5.23</v>
       </c>
       <c r="E9" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>5.23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>3</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" t="s">
+        <v>116</v>
+      </c>
+      <c r="M9" s="2">
+        <v>18.989999999999998</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>18.989999999999998</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="U9" s="2"/>
+      <c r="V9" s="5"/>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -936,64 +1209,98 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2">
         <v>3.63</v>
       </c>
       <c r="E10" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>3.63</v>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0.5</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10" t="s">
-        <v>64</v>
-      </c>
-      <c r="J10">
-        <v>1</v>
-      </c>
-      <c r="K10" s="2">
-        <v>2</v>
-      </c>
-      <c r="L10" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>2</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="H10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" t="s">
+        <v>114</v>
+      </c>
+      <c r="M10" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+      <c r="O10" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>7.99</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+      <c r="V10" s="2"/>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="2">
-        <v>1.92</v>
+        <v>0.99</v>
       </c>
       <c r="E11" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>1.92</v>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>1.98</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M11" s="2"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
+        <v>120</v>
+      </c>
+      <c r="M11" s="2">
+        <v>11.99</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+      <c r="O11" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>11.99</v>
+      </c>
+      <c r="P11" t="s">
+        <v>87</v>
+      </c>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+    </row>
+    <row r="12" spans="1:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1005,50 +1312,85 @@
         <v>4.33</v>
       </c>
       <c r="E12" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>4.33</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="2">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="L12" t="s">
+        <v>117</v>
+      </c>
+      <c r="M12" s="2">
+        <v>14.99</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+      <c r="O12" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>14.99</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="D13" s="2">
         <v>1.8</v>
       </c>
       <c r="E13" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>1.8</v>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L13" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" t="s">
+        <v>109</v>
+      </c>
+      <c r="M13" s="2">
+        <v>11.35</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+      <c r="O13" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>11.35</v>
+      </c>
+      <c r="P13" t="s">
+        <v>99</v>
+      </c>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1060,21 +1402,37 @@
         <v>2.34</v>
       </c>
       <c r="E14" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>2.34</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0</v>
+      </c>
+      <c r="L14" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14" s="2">
+        <v>8.89</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>17.78</v>
+      </c>
+      <c r="P14" t="s">
+        <v>113</v>
+      </c>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1086,47 +1444,88 @@
         <v>3.82</v>
       </c>
       <c r="E15" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>3.82</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M15" s="2"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
+        <v>121</v>
+      </c>
+      <c r="M15" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>9.5</v>
+      </c>
+      <c r="P15" t="s">
+        <v>95</v>
+      </c>
+      <c r="U15" s="2"/>
+      <c r="V15" s="2"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D16" s="2">
         <v>0.79</v>
       </c>
       <c r="E16" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>0.79</v>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>1.03</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L16" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M16" s="2"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1.03</v>
+      </c>
+      <c r="K16" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" t="s">
+        <v>122</v>
+      </c>
+      <c r="M16" s="2">
+        <v>8.99</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+      <c r="O16" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>8.99</v>
+      </c>
+      <c r="P16" t="s">
+        <v>98</v>
+      </c>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1138,21 +1537,37 @@
         <v>0.46</v>
       </c>
       <c r="E17" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>0.46</v>
       </c>
-      <c r="F17" t="s">
-        <v>33</v>
-      </c>
-      <c r="L17" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="2"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>101</v>
+      </c>
+      <c r="M17" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>19.98</v>
+      </c>
+      <c r="P17" t="s">
+        <v>100</v>
+      </c>
+      <c r="U17" s="2"/>
+      <c r="V17" s="2"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1164,21 +1579,37 @@
         <v>7.99</v>
       </c>
       <c r="E18" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>7.99</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L18" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M18" s="2"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
+        <v>123</v>
+      </c>
+      <c r="M18" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>9.99</v>
+      </c>
+      <c r="P18" t="s">
+        <v>86</v>
+      </c>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1190,47 +1621,88 @@
         <v>15.19</v>
       </c>
       <c r="E19" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>15.19</v>
       </c>
       <c r="F19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
+        <v>93</v>
+      </c>
+      <c r="M19" s="2">
+        <v>25.99</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>51.98</v>
+      </c>
+      <c r="P19" t="s">
+        <v>88</v>
+      </c>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="L19" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>38</v>
-      </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D20" s="2">
         <v>16</v>
       </c>
       <c r="E20" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>4.88</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" t="s">
+        <v>74</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" s="2">
+        <v>4.88</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L20" t="s">
+        <v>93</v>
+      </c>
+      <c r="M20" s="2">
         <v>16</v>
       </c>
-      <c r="F20" t="s">
+      <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>16</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>39</v>
-      </c>
-      <c r="L20" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M20" s="2"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>41</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1242,21 +1714,37 @@
         <v>1</v>
       </c>
       <c r="E21" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>43</v>
-      </c>
-      <c r="L21" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M21" s="2"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>109</v>
+      </c>
+      <c r="M21" s="2">
+        <v>5.95</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>5.95</v>
+      </c>
+      <c r="P21" t="s">
+        <v>83</v>
+      </c>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1268,21 +1756,37 @@
         <v>1</v>
       </c>
       <c r="E22" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>1</v>
       </c>
       <c r="F22" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>109</v>
+      </c>
+      <c r="M22" s="2">
+        <v>6.42</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>6.42</v>
+      </c>
+      <c r="P22" t="s">
+        <v>84</v>
+      </c>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>43</v>
-      </c>
-      <c r="L22" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M22" s="2"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>45</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1294,21 +1798,37 @@
         <v>0.79</v>
       </c>
       <c r="E23" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>0.79</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L23" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>110</v>
+      </c>
+      <c r="M23" s="2">
+        <v>5.99</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>5.99</v>
+      </c>
+      <c r="P23" t="s">
+        <v>111</v>
+      </c>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1320,21 +1840,37 @@
         <v>0.73</v>
       </c>
       <c r="E24" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>0.73</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
-      </c>
-      <c r="L24" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>53</v>
+      </c>
+      <c r="M24" s="2">
+        <v>11.49</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>11.49</v>
+      </c>
+      <c r="P24" t="s">
+        <v>102</v>
+      </c>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1346,99 +1882,160 @@
         <v>0.15</v>
       </c>
       <c r="E25" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>0.3</v>
       </c>
       <c r="F25" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0</v>
+      </c>
+      <c r="L25" t="s">
+        <v>108</v>
+      </c>
+      <c r="M25" s="2">
+        <v>6.9</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>6.9</v>
+      </c>
+      <c r="P25" t="s">
+        <v>90</v>
+      </c>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>48</v>
       </c>
-      <c r="L25" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M25" s="2"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>50</v>
-      </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2">
         <v>2.86</v>
       </c>
       <c r="E26" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>2.86</v>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>51</v>
-      </c>
-      <c r="L26" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="2"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
+        <v>96</v>
+      </c>
+      <c r="M26" s="2">
+        <v>12.69</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>12.69</v>
+      </c>
+      <c r="P26" t="s">
+        <v>97</v>
+      </c>
+      <c r="U26" s="2"/>
+      <c r="V26" s="2"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="D27" s="2">
         <v>2.31</v>
       </c>
       <c r="E27" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>2.31</v>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0</v>
       </c>
       <c r="F27" t="s">
+        <v>49</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="L27" t="s">
+        <v>119</v>
+      </c>
+      <c r="M27" s="2">
+        <v>7.99</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>7.99</v>
+      </c>
+      <c r="P27" t="s">
+        <v>91</v>
+      </c>
+      <c r="U27" s="2"/>
+      <c r="V27" s="2"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>51</v>
       </c>
-      <c r="L27" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M27" s="2"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>53</v>
-      </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="D28" s="2">
         <v>1.38</v>
       </c>
       <c r="E28" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
-        <v>1.38</v>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>51</v>
-      </c>
-      <c r="L28" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M28" s="2"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
+        <v>105</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+      <c r="O28" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>0</v>
+      </c>
+      <c r="U28" s="2"/>
+      <c r="V28" s="2"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1450,21 +2047,37 @@
         <v>9.99</v>
       </c>
       <c r="E29" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>9.99</v>
       </c>
       <c r="F29" t="s">
-        <v>56</v>
-      </c>
-      <c r="L29" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M29" s="2"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0</v>
+      </c>
+      <c r="L29" t="s">
+        <v>106</v>
+      </c>
+      <c r="M29" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+      <c r="O29" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>9.99</v>
+      </c>
+      <c r="P29" t="s">
+        <v>107</v>
+      </c>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1476,42 +2089,97 @@
         <v>7.99</v>
       </c>
       <c r="E30" s="2">
-        <f>IF( Table1[[#This Row],[Substitute]] = "Yes", Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] )</f>
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
         <v>7.99</v>
       </c>
-      <c r="F30" t="s">
-        <v>68</v>
+      <c r="F30" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="G30" t="s">
-        <v>67</v>
-      </c>
-      <c r="L30" s="2">
-        <f>Table2[[#This Row],[Quantity]]*Table2[[#This Row],[Unit Price]]</f>
-        <v>0</v>
-      </c>
-      <c r="M30" s="2"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0</v>
+      </c>
+      <c r="L30" t="s">
+        <v>103</v>
+      </c>
+      <c r="M30" s="2">
+        <v>9.99</v>
+      </c>
+      <c r="N30">
+        <v>2</v>
+      </c>
+      <c r="O30" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>19.98</v>
+      </c>
+      <c r="P30" t="s">
+        <v>104</v>
+      </c>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2</v>
+      </c>
+      <c r="E31" s="2">
+        <f>IF( Table1[[#This Row],[Substitute]]="OBE", 0, IF( Table1[[#This Row],[Substitute]] = "Yes", Table1[[#This Row],[Alt Quantity]]*Table1[[#This Row],[Sub Unit Price]], Table1[[#This Row],[Quantity]]*Table1[[#This Row],[Unit Price]] ))</f>
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>72</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="L31" t="s">
+        <v>105</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31" s="2">
+        <f>Table1[[#This Row],[Amazon / What I Used Price]]*Table1[[#This Row],[Amazon Quantity]]</f>
+        <v>0</v>
+      </c>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E32" s="2">
         <f>SUBTOTAL(109,Table1[Total])</f>
-        <v>91.85</v>
-      </c>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+        <v>85.83</v>
+      </c>
+      <c r="O32" s="2">
+        <f>SUBTOTAL(109,Table1[Amazon Total Price])</f>
+        <v>311.88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C30" xr:uid="{85C47236-C204-4451-A361-76C1023E370E}">
-      <formula1>"Yes,No,N/A"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31" xr:uid="{6436DCCA-0471-409C-90F8-71260F5AE877}">
+      <formula1>"Yes,No,N/A,OBE"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -1524,16 +2192,21 @@
     <hyperlink ref="F16" r:id="rId7" xr:uid="{9BBF8E1D-3BBF-4D29-B586-53B80FFEB964}"/>
     <hyperlink ref="F23" r:id="rId8" xr:uid="{B625AE6A-7AC1-4FE4-A8A1-071D6B1F0A12}"/>
     <hyperlink ref="F19" r:id="rId9" xr:uid="{CE7E51FD-7FB0-406D-A849-52CAE3CB66FE}"/>
-    <hyperlink ref="M2" r:id="rId10" display="https://www.aliexpress.com/item/32995552535.html" xr:uid="{FEA8649C-928C-418F-809A-0C9F57312B6C}"/>
-    <hyperlink ref="M3" r:id="rId11" xr:uid="{9A43F33D-8180-4820-A35E-600177C68E41}"/>
-    <hyperlink ref="M9" r:id="rId12" xr:uid="{F8C58054-AD11-450A-9683-740C11C40AD1}"/>
-    <hyperlink ref="F18" r:id="rId13" xr:uid="{9B7A094D-A856-4D13-8D26-A8B9C6733471}"/>
+    <hyperlink ref="F18" r:id="rId10" xr:uid="{9B7A094D-A856-4D13-8D26-A8B9C6733471}"/>
+    <hyperlink ref="K3" r:id="rId11" xr:uid="{CBF1C379-6CB2-432D-816B-E7697F854A00}"/>
+    <hyperlink ref="K9" r:id="rId12" xr:uid="{5B9BEFE2-36DC-4418-883F-E62D9291E02D}"/>
+    <hyperlink ref="K10" r:id="rId13" xr:uid="{DFB798B1-D372-49CD-976E-C391876800BB}"/>
+    <hyperlink ref="K20" r:id="rId14" xr:uid="{A2527BC6-92D3-4979-B27A-58C787F7A51B}"/>
+    <hyperlink ref="F30" r:id="rId15" xr:uid="{39E8CD9E-AA70-4C5A-A1AA-3929EAF4BEA8}"/>
+    <hyperlink ref="F20" r:id="rId16" xr:uid="{560417EB-FE9E-473F-9B42-97208F192E99}"/>
+    <hyperlink ref="P20" r:id="rId17" xr:uid="{9014AFFF-3522-4C71-92DF-2565DEDC41BD}"/>
+    <hyperlink ref="F17" r:id="rId18" xr:uid="{B00D8416-BB24-490D-8076-6B382128AA60}"/>
+    <hyperlink ref="P9" r:id="rId19" xr:uid="{5D17342A-F858-441A-BD76-F4EB4B270E67}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
-  <tableParts count="2">
-    <tablePart r:id="rId15"/>
-    <tablePart r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
+  <tableParts count="1">
+    <tablePart r:id="rId21"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>